<commit_message>
fix: correct Gemini CoT table
</commit_message>
<xml_diff>
--- a/data/benchmarks/sample_comparison.xlsx
+++ b/data/benchmarks/sample_comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seren\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seren\Desktop\Università Magistrale SICUREZZA DEI SISTEMI SOFTWARE\Secondo Anno\Semantic Analytics For Cybersecurity\Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BE8B76-9263-4399-A9F1-249C8898635F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F967C526-E014-4EB1-9005-725E024844B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5976" yWindow="1968" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>0.7222</t>
   </si>
   <si>
-    <t>0.0247</t>
-  </si>
-  <si>
     <t>0.7531</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>0.8333</t>
+  </si>
+  <si>
+    <t>0.5617</t>
   </si>
 </sst>
 </file>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,13 +669,13 @@
         <v>11</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -849,7 +849,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>11</v>
@@ -861,13 +861,13 @@
         <v>11</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -973,13 +973,13 @@
         <v>9</v>
       </c>
       <c r="C25" s="6">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>9</v>
@@ -1005,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="6">
-        <v>158</v>
+        <v>71</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>10</v>
@@ -1037,31 +1037,31 @@
         <v>11</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>